<commit_message>
new: calculating the electrolyte concentration based on the ion concentrations
</commit_message>
<xml_diff>
--- a/atmPy/aerosols/materials/materials.xlsx
+++ b/atmPy/aerosols/materials/materials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23540"/>
+    <workbookView xWindow="-32760" yWindow="0" windowWidth="38400" windowHeight="23540"/>
   </bookViews>
   <sheets>
     <sheet name="page 1" sheetId="1" r:id="rId1"/>
@@ -51,12 +51,66 @@
         </r>
       </text>
     </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">Hagen Telg:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>when desolved in water:
+what is the cation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Hagen Telg:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+when desolved in water:
+what is the anion</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
   <si>
     <t>Species</t>
   </si>
@@ -179,13 +233,106 @@
   </si>
   <si>
     <t>ammonium_sulfate</t>
+  </si>
+  <si>
+    <t>Na2SO4</t>
+  </si>
+  <si>
+    <t>NaNO3</t>
+  </si>
+  <si>
+    <t>NaCl</t>
+  </si>
+  <si>
+    <t>Ca(NO3)2</t>
+  </si>
+  <si>
+    <t>CaCl2</t>
+  </si>
+  <si>
+    <t>H^+</t>
+  </si>
+  <si>
+    <t>NH4^+</t>
+  </si>
+  <si>
+    <t>Na^+</t>
+  </si>
+  <si>
+    <t>Ca^2+</t>
+  </si>
+  <si>
+    <t>SO4^2-</t>
+  </si>
+  <si>
+    <t>NO3^-</t>
+  </si>
+  <si>
+    <t>Cl^-</t>
+  </si>
+  <si>
+    <t>ammonium</t>
+  </si>
+  <si>
+    <t>sulfate</t>
+  </si>
+  <si>
+    <t>nitrate</t>
+  </si>
+  <si>
+    <t>chloride</t>
+  </si>
+  <si>
+    <t>ion</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>an</t>
+  </si>
+  <si>
+    <t>anion</t>
+  </si>
+  <si>
+    <t>cation</t>
+  </si>
+  <si>
+    <t>proton</t>
+  </si>
+  <si>
+    <t>molecular_weight</t>
+  </si>
+  <si>
+    <t>charge_on_ion</t>
+  </si>
+  <si>
+    <t>sodium_chloride</t>
+  </si>
+  <si>
+    <t>sodium</t>
+  </si>
+  <si>
+    <t>sodium_sulfate</t>
+  </si>
+  <si>
+    <t>sodium_nitrate</t>
+  </si>
+  <si>
+    <t>calcium_nitrate</t>
+  </si>
+  <si>
+    <t>calcium_chloride</t>
+  </si>
+  <si>
+    <t>calcium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -216,6 +363,22 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -272,8 +435,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -303,7 +494,35 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="29">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -596,26 +815,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="21.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="52" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="48.83203125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="3"/>
+    <col min="5" max="5" width="18.1640625" style="3" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="52" style="3" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1">
+    <row r="1" spans="1:13" ht="28" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -640,8 +860,23 @@
       <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1">
+      <c r="I1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -667,7 +902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1">
+    <row r="3" spans="1:13" ht="18" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -693,7 +928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1">
+    <row r="4" spans="1:13" ht="18" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -718,8 +953,14 @@
       <c r="H4" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1">
+      <c r="L4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
@@ -745,7 +986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1">
+    <row r="6" spans="1:13" ht="18" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -771,7 +1012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1">
+    <row r="7" spans="1:13" ht="18" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
@@ -796,8 +1037,17 @@
       <c r="H7" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="18" customHeight="1">
+      <c r="I7" s="3">
+        <v>132</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="18" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
@@ -822,8 +1072,17 @@
       <c r="H8" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1">
+      <c r="I8" s="3">
+        <v>63</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="18" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>27</v>
       </c>
@@ -848,8 +1107,17 @@
       <c r="H9" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1">
+      <c r="I9" s="3">
+        <v>80</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="18" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -874,8 +1142,17 @@
       <c r="H10" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1">
+      <c r="I10" s="3">
+        <v>36.5</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="18" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>28</v>
       </c>
@@ -900,10 +1177,223 @@
       <c r="H11" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1"/>
+      <c r="I11" s="3">
+        <v>53.5</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="18" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="3">
+        <v>142</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="3">
+        <v>85</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="3">
+        <v>58.5</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="3">
+        <v>164</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I16" s="3">
+        <v>111</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" s="3">
+        <v>18</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" s="3">
+        <v>23</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" s="3">
+        <v>40</v>
+      </c>
+      <c r="J20" s="3">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="3">
+        <v>96</v>
+      </c>
+      <c r="J21" s="3">
+        <v>2</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" s="3">
+        <v>62</v>
+      </c>
+      <c r="J22" s="3">
+        <v>1</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="3">
+        <v>35.5</v>
+      </c>
+      <c r="J23" s="3">
+        <v>1</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
new: apply mixing rules to calculate kappa from chemical composition
</commit_message>
<xml_diff>
--- a/atmPy/aerosols/materials/materials.xlsx
+++ b/atmPy/aerosols/materials/materials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-32760" yWindow="0" windowWidth="38400" windowHeight="23540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33000" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="page 1" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
   <si>
     <t>Species</t>
   </si>
@@ -326,6 +326,9 @@
   </si>
   <si>
     <t>calcium</t>
+  </si>
+  <si>
+    <t>hydrogen_sulfate</t>
   </si>
 </sst>
 </file>
@@ -817,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -827,10 +830,10 @@
     <col min="2" max="2" width="29.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="21.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" style="3" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="52" style="3" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="3" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="32.33203125" style="3" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="52" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" style="3" customWidth="1"/>
     <col min="10" max="16384" width="8.83203125" style="3"/>
   </cols>
@@ -953,6 +956,9 @@
       <c r="H4" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="I4" s="3">
+        <v>98</v>
+      </c>
       <c r="L4" s="3" t="s">
         <v>62</v>
       </c>
@@ -984,6 +990,15 @@
       </c>
       <c r="H5" s="6" t="s">
         <v>5</v>
+      </c>
+      <c r="I5" s="3">
+        <v>115</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1">

</xml_diff>

<commit_message>
change: new value for kappa organic
</commit_message>
<xml_diff>
--- a/atmPy/aerosols/materials/materials.xlsx
+++ b/atmPy/aerosols/materials/materials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33000" windowHeight="20540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33800" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="page 1" sheetId="1" r:id="rId1"/>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -919,7 +919,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="6">
-        <v>7.5999999999999998E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
some new materials mainly for dust
</commit_message>
<xml_diff>
--- a/atmPy/aerosols/materials/materials.xlsx
+++ b/atmPy/aerosols/materials/materials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-32740" yWindow="-80" windowWidth="33800" windowHeight="20620"/>
+    <workbookView xWindow="-33140" yWindow="0" windowWidth="32740" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="page 1" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="79">
   <si>
     <t>Species</t>
   </si>
@@ -329,6 +329,24 @@
   </si>
   <si>
     <t>hydrogen_sulfate</t>
+  </si>
+  <si>
+    <t>Polystyrene</t>
+  </si>
+  <si>
+    <t>wikipedia</t>
+  </si>
+  <si>
+    <t>Silicon dioxide</t>
+  </si>
+  <si>
+    <t>Aluminium oxide</t>
+  </si>
+  <si>
+    <t>Handbook of Mineralogy. Volume III: Halides, Hydroxides, Oxides</t>
+  </si>
+  <si>
+    <t>MgCl</t>
   </si>
 </sst>
 </file>
@@ -438,7 +456,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -468,8 +486,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -499,6 +518,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="29" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -514,7 +536,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="30">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -543,6 +565,7 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -835,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -846,10 +869,10 @@
     <col min="1" max="1" width="13.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28" style="3" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="52" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="17" customWidth="1"/>
     <col min="8" max="8" width="32.33203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" style="3" customWidth="1"/>
     <col min="10" max="16384" width="8.83203125" style="3"/>
@@ -874,7 +897,7 @@
       <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -915,7 +938,7 @@
       <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="13">
         <v>1</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -941,7 +964,7 @@
       <c r="F3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="14">
         <v>1.4</v>
       </c>
       <c r="H3" s="6" t="s">
@@ -967,7 +990,7 @@
       <c r="F4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="14">
         <v>1.8</v>
       </c>
       <c r="H4" s="6" t="s">
@@ -1002,7 +1025,7 @@
       <c r="F5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="14">
         <v>1.78</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -1037,7 +1060,7 @@
       <c r="F6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="14">
         <v>1.83</v>
       </c>
       <c r="H6" s="6" t="s">
@@ -1063,7 +1086,7 @@
       <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="14">
         <v>1.76</v>
       </c>
       <c r="H7" s="7" t="s">
@@ -1098,7 +1121,7 @@
       <c r="F8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="14">
         <v>1.5128999999999999</v>
       </c>
       <c r="H8" s="7" t="s">
@@ -1133,7 +1156,7 @@
       <c r="F9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="14">
         <v>1.7250000000000001</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -1168,7 +1191,7 @@
       <c r="F10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="14">
         <v>1.49</v>
       </c>
       <c r="H10" s="6" t="s">
@@ -1203,7 +1226,7 @@
       <c r="F11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="15">
         <v>1.5189999999999999</v>
       </c>
       <c r="H11" s="8" t="s">
@@ -1226,11 +1249,17 @@
       <c r="B12" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="15">
+      <c r="C12">
+        <v>1.468</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="16">
         <v>2.6640000000000001</v>
       </c>
-      <c r="H12" s="10">
-        <v>2.6640000000000001</v>
+      <c r="H12" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="I12" s="3">
         <v>142</v>
@@ -1249,8 +1278,17 @@
       <c r="B13" s="3" t="s">
         <v>68</v>
       </c>
+      <c r="C13">
+        <v>1.587</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="G13">
         <v>2.2570000000000001</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="I13" s="3">
         <v>85</v>
@@ -1269,11 +1307,17 @@
       <c r="B14" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="C14">
+        <v>1.5442</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="G14">
         <v>2.165</v>
       </c>
-      <c r="H14" s="10">
-        <v>2.165</v>
+      <c r="H14" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="I14" s="3">
         <v>58.5</v>
@@ -1295,6 +1339,9 @@
       <c r="G15">
         <v>2.504</v>
       </c>
+      <c r="H15" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="I15" s="3">
         <v>164</v>
       </c>
@@ -1312,9 +1359,18 @@
       <c r="B16" t="s">
         <v>70</v>
       </c>
+      <c r="C16" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="G16">
         <v>2.15</v>
       </c>
+      <c r="H16" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="I16" s="3">
         <v>111</v>
       </c>
@@ -1330,124 +1386,171 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="3">
-        <v>1</v>
-      </c>
-      <c r="J17" s="3">
-        <v>1</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>58</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B17"/>
+      <c r="D17" s="10"/>
+      <c r="G17"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="3">
-        <v>18</v>
-      </c>
-      <c r="J18" s="3">
-        <v>1</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" s="3">
-        <v>23</v>
-      </c>
-      <c r="J19" s="3">
-        <v>1</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="B18"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:11" ht="28">
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1.5489999999999999</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20" s="3">
-        <v>40</v>
-      </c>
-      <c r="J20" s="3">
-        <v>2</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1.766</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="I21" s="3">
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="J21" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I22" s="3">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="J22" s="3">
         <v>1</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="I23" s="3">
-        <v>35.5</v>
+        <v>23</v>
       </c>
       <c r="J23" s="3">
         <v>1</v>
       </c>
       <c r="K23" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" s="3">
+        <v>40</v>
+      </c>
+      <c r="J24" s="3">
+        <v>2</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" s="3">
+        <v>96</v>
+      </c>
+      <c r="J25" s="3">
+        <v>2</v>
+      </c>
+      <c r="K25" s="3" t="s">
         <v>59</v>
       </c>
     </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" s="3">
+        <v>62</v>
+      </c>
+      <c r="J26" s="3">
+        <v>1</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="3">
+        <v>35.5</v>
+      </c>
+      <c r="J27" s="3">
+        <v>1</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="17">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D19" r:id="rId1" display="https://www.mindat.org/min-3337.html"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>